<commit_message>
Updated Excel file with new data
</commit_message>
<xml_diff>
--- a/Forecaster_results.xlsx
+++ b/Forecaster_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
   <si>
     <t>Input Sample Date</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>2024-02-21</t>
+  </si>
+  <si>
+    <t>2024-02-22</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -712,385 +715,32 @@
         <v>58280.859375</v>
       </c>
     </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>53409.74609375</v>
+      </c>
+      <c r="C16">
+        <v>54860.8828125</v>
+      </c>
+      <c r="D16">
+        <v>55706.15234375</v>
+      </c>
+      <c r="E16">
+        <v>55990.953125</v>
+      </c>
+      <c r="F16">
+        <v>57094.24609375</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>51392.23046875</v>
-      </c>
-      <c r="C2">
-        <v>49972.68359375</v>
-      </c>
-      <c r="D2">
-        <v>51072.9296875</v>
-      </c>
-      <c r="E2">
-        <v>54902.2578125</v>
-      </c>
-      <c r="F2">
-        <v>55231.94140625</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>51392.23046875</v>
-      </c>
-      <c r="C3">
-        <v>49972.68359375</v>
-      </c>
-      <c r="D3">
-        <v>51072.9296875</v>
-      </c>
-      <c r="E3">
-        <v>54902.2578125</v>
-      </c>
-      <c r="F3">
-        <v>55231.94140625</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>51392.23046875</v>
-      </c>
-      <c r="C4">
-        <v>49972.68359375</v>
-      </c>
-      <c r="D4">
-        <v>51072.9296875</v>
-      </c>
-      <c r="E4">
-        <v>54902.2578125</v>
-      </c>
-      <c r="F4">
-        <v>55231.94140625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>51392.23046875</v>
-      </c>
-      <c r="C5">
-        <v>49972.68359375</v>
-      </c>
-      <c r="D5">
-        <v>51072.9296875</v>
-      </c>
-      <c r="E5">
-        <v>54902.2578125</v>
-      </c>
-      <c r="F5">
-        <v>55231.94140625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C6">
-        <v>52312.09375</v>
-      </c>
-      <c r="D6">
-        <v>52734.28515625</v>
-      </c>
-      <c r="E6">
-        <v>54746.88671875</v>
-      </c>
-      <c r="F6">
-        <v>55604.62890625</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>50117.4375</v>
-      </c>
-      <c r="C7">
-        <v>49500.765625</v>
-      </c>
-      <c r="D7">
-        <v>49463.6484375</v>
-      </c>
-      <c r="E7">
-        <v>53064.609375</v>
-      </c>
-      <c r="F7">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C8">
-        <v>52312.09375</v>
-      </c>
-      <c r="D8">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E8">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F8">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C9">
-        <v>52312.09375</v>
-      </c>
-      <c r="D9">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E9">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F9">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C10">
-        <v>52312.09375</v>
-      </c>
-      <c r="D10">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E10">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F10">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C11">
-        <v>52312.09375</v>
-      </c>
-      <c r="D11">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E11">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F11">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C12">
-        <v>52312.09375</v>
-      </c>
-      <c r="D12">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E12">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F12">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C13">
-        <v>52312.09375</v>
-      </c>
-      <c r="D13">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E13">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F13">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C14">
-        <v>52312.09375</v>
-      </c>
-      <c r="D14">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E14">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F14">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C15">
-        <v>52312.09375</v>
-      </c>
-      <c r="D15">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E15">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F15">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C16">
-        <v>52312.09375</v>
-      </c>
-      <c r="D16">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E16">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F16">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>52899.53515625</v>
-      </c>
-      <c r="C17">
-        <v>52312.09375</v>
-      </c>
-      <c r="D17">
-        <v>51522.24609375</v>
-      </c>
-      <c r="E17">
-        <v>53303.03515625</v>
-      </c>
-      <c r="F17">
-        <v>54405.50390625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18">
-        <v>50255.06640625</v>
-      </c>
-      <c r="C18">
-        <v>49737.80078125</v>
-      </c>
-      <c r="D18">
-        <v>49581.58203125</v>
-      </c>
-      <c r="E18">
-        <v>53358.05859375</v>
-      </c>
-      <c r="F18">
-        <v>54398.640625</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -1123,19 +773,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>55456.14453125</v>
+        <v>51392.23046875</v>
       </c>
       <c r="C2">
-        <v>53955.640625</v>
+        <v>49972.68359375</v>
       </c>
       <c r="D2">
-        <v>54523.71875</v>
+        <v>51072.9296875</v>
       </c>
       <c r="E2">
-        <v>58003.41015625</v>
+        <v>54902.2578125</v>
       </c>
       <c r="F2">
-        <v>58096.3984375</v>
+        <v>55231.94140625</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1143,19 +793,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>55456.14453125</v>
+        <v>51392.23046875</v>
       </c>
       <c r="C3">
-        <v>53955.640625</v>
+        <v>49972.68359375</v>
       </c>
       <c r="D3">
-        <v>54523.71875</v>
+        <v>51072.9296875</v>
       </c>
       <c r="E3">
-        <v>58003.41015625</v>
+        <v>54902.2578125</v>
       </c>
       <c r="F3">
-        <v>58096.3984375</v>
+        <v>55231.94140625</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1163,19 +813,19 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>55456.14453125</v>
+        <v>51392.23046875</v>
       </c>
       <c r="C4">
-        <v>53955.640625</v>
+        <v>49972.68359375</v>
       </c>
       <c r="D4">
-        <v>54523.71875</v>
+        <v>51072.9296875</v>
       </c>
       <c r="E4">
-        <v>58003.41015625</v>
+        <v>54902.2578125</v>
       </c>
       <c r="F4">
-        <v>58096.3984375</v>
+        <v>55231.94140625</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1183,19 +833,19 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>55456.14453125</v>
+        <v>51392.23046875</v>
       </c>
       <c r="C5">
-        <v>53955.640625</v>
+        <v>49972.68359375</v>
       </c>
       <c r="D5">
-        <v>54523.71875</v>
+        <v>51072.9296875</v>
       </c>
       <c r="E5">
-        <v>58003.41015625</v>
+        <v>54902.2578125</v>
       </c>
       <c r="F5">
-        <v>58096.3984375</v>
+        <v>55231.94140625</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1203,19 +853,19 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C6">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D6">
-        <v>56626.20703125</v>
+        <v>52734.28515625</v>
       </c>
       <c r="E6">
-        <v>57908.1015625</v>
+        <v>54746.88671875</v>
       </c>
       <c r="F6">
-        <v>57216.00390625</v>
+        <v>55604.62890625</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1223,19 +873,19 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>52796.4765625</v>
+        <v>50117.4375</v>
       </c>
       <c r="C7">
-        <v>52790.82421875</v>
+        <v>49500.765625</v>
       </c>
       <c r="D7">
-        <v>53097.16796875</v>
+        <v>49463.6484375</v>
       </c>
       <c r="E7">
-        <v>56762.5546875</v>
+        <v>53064.609375</v>
       </c>
       <c r="F7">
-        <v>55459.37109375</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1243,19 +893,19 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C8">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D8">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E8">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F8">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1263,19 +913,19 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C9">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D9">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E9">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F9">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1283,19 +933,19 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C10">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D10">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E10">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F10">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1303,19 +953,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C11">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D11">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E11">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F11">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1323,19 +973,19 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C12">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D12">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E12">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F12">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1343,19 +993,19 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C13">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D13">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E13">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F13">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1363,19 +1013,19 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C14">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D14">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E14">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F14">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1383,19 +1033,19 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C15">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D15">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E15">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F15">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1403,19 +1053,19 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C16">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D16">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E16">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F16">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1423,19 +1073,19 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>55046.73046875</v>
+        <v>52899.53515625</v>
       </c>
       <c r="C17">
-        <v>56418.20703125</v>
+        <v>52312.09375</v>
       </c>
       <c r="D17">
-        <v>55733.4921875</v>
+        <v>51522.24609375</v>
       </c>
       <c r="E17">
-        <v>56780.1171875</v>
+        <v>53303.03515625</v>
       </c>
       <c r="F17">
-        <v>57295.6953125</v>
+        <v>54405.50390625</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1443,6 +1093,399 @@
         <v>10</v>
       </c>
       <c r="B18">
+        <v>50255.06640625</v>
+      </c>
+      <c r="C18">
+        <v>49737.80078125</v>
+      </c>
+      <c r="D18">
+        <v>49581.58203125</v>
+      </c>
+      <c r="E18">
+        <v>53358.05859375</v>
+      </c>
+      <c r="F18">
+        <v>54398.640625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>51660.63671875</v>
+      </c>
+      <c r="C19">
+        <v>50626.66796875</v>
+      </c>
+      <c r="D19">
+        <v>49251.078125</v>
+      </c>
+      <c r="E19">
+        <v>53215.46875</v>
+      </c>
+      <c r="F19">
+        <v>54772.078125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>55456.14453125</v>
+      </c>
+      <c r="C2">
+        <v>53955.640625</v>
+      </c>
+      <c r="D2">
+        <v>54523.71875</v>
+      </c>
+      <c r="E2">
+        <v>58003.41015625</v>
+      </c>
+      <c r="F2">
+        <v>58096.3984375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>55456.14453125</v>
+      </c>
+      <c r="C3">
+        <v>53955.640625</v>
+      </c>
+      <c r="D3">
+        <v>54523.71875</v>
+      </c>
+      <c r="E3">
+        <v>58003.41015625</v>
+      </c>
+      <c r="F3">
+        <v>58096.3984375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>55456.14453125</v>
+      </c>
+      <c r="C4">
+        <v>53955.640625</v>
+      </c>
+      <c r="D4">
+        <v>54523.71875</v>
+      </c>
+      <c r="E4">
+        <v>58003.41015625</v>
+      </c>
+      <c r="F4">
+        <v>58096.3984375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>55456.14453125</v>
+      </c>
+      <c r="C5">
+        <v>53955.640625</v>
+      </c>
+      <c r="D5">
+        <v>54523.71875</v>
+      </c>
+      <c r="E5">
+        <v>58003.41015625</v>
+      </c>
+      <c r="F5">
+        <v>58096.3984375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C6">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D6">
+        <v>56626.20703125</v>
+      </c>
+      <c r="E6">
+        <v>57908.1015625</v>
+      </c>
+      <c r="F6">
+        <v>57216.00390625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>52796.4765625</v>
+      </c>
+      <c r="C7">
+        <v>52790.82421875</v>
+      </c>
+      <c r="D7">
+        <v>53097.16796875</v>
+      </c>
+      <c r="E7">
+        <v>56762.5546875</v>
+      </c>
+      <c r="F7">
+        <v>55459.37109375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C8">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D8">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E8">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F8">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C9">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D9">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E9">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F9">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C10">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D10">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E10">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F10">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C11">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D11">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E11">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F11">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C12">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D12">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E12">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F12">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C13">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D13">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E13">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F13">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C14">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D14">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E14">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F14">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C15">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D15">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E15">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F15">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C16">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D16">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E16">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F16">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>55046.73046875</v>
+      </c>
+      <c r="C17">
+        <v>56418.20703125</v>
+      </c>
+      <c r="D17">
+        <v>55733.4921875</v>
+      </c>
+      <c r="E17">
+        <v>56780.1171875</v>
+      </c>
+      <c r="F17">
+        <v>57295.6953125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
         <v>52835.66015625</v>
       </c>
       <c r="C18">
@@ -1476,6 +1519,26 @@
       </c>
       <c r="F19">
         <v>56757.0390625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>54590.59375</v>
+      </c>
+      <c r="C20">
+        <v>53823.20703125</v>
+      </c>
+      <c r="D20">
+        <v>53286.18359375</v>
+      </c>
+      <c r="E20">
+        <v>56140.96484375</v>
+      </c>
+      <c r="F20">
+        <v>54841.17578125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>